<commit_message>
Feat: PandasPractice first approach
</commit_message>
<xml_diff>
--- a/Car_Sales_Kaggle_DV0130EN_Lab1_Start.xlsx
+++ b/Car_Sales_Kaggle_DV0130EN_Lab1_Start.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DataAnalysisPath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A4C507-C9D7-46A4-90E7-800E02DA9CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF88D29-C0A0-4B48-82EE-1EDBCE26E5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1283,40 +1283,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
+  <dxfs count="73">
     <dxf>
       <font>
         <b/>
@@ -11532,7 +11499,7 @@
     <dataField name="Average of Retention %" fld="6" subtotal="average" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="83">
+    <format dxfId="72">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -11544,10 +11511,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="71">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -12194,7 +12161,7 @@
     <dataField name="Average of Price" fld="4" subtotal="average" baseField="0" baseItem="78" numFmtId="167"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="80">
+    <format dxfId="69">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -12203,7 +12170,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -12212,7 +12179,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="67">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -12221,7 +12188,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -12282,7 +12249,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1D2600A8-6634-4642-AAD2-0860E46FD306}" name="Table14" displayName="Table14" ref="A1:S156" totalsRowShown="0" headerRowDxfId="76" headerRowCellStyle="60% - Accent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1D2600A8-6634-4642-AAD2-0860E46FD306}" name="Table14" displayName="Table14" ref="A1:S156" totalsRowShown="0" headerRowDxfId="65" headerRowCellStyle="60% - Accent1">
   <autoFilter ref="A1:S156" xr:uid="{142A1155-8F99-4580-8274-3FFCD265F860}">
     <filterColumn colId="0">
       <filters>
@@ -12294,38 +12261,38 @@
     <sortCondition ref="B1:B156"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="2" xr3:uid="{CCFD9DCD-33DA-4C1C-B39D-1F8C0CA940C0}" name="Manufacturer" dataDxfId="75" dataCellStyle="60% - Accent2"/>
-    <tableColumn id="1" xr3:uid="{91732ACF-B59B-4736-A06E-BE7ADB4669C2}" name="Model" dataDxfId="74" dataCellStyle="60% - Accent6"/>
-    <tableColumn id="4" xr3:uid="{AC38EB39-9FE7-4815-9A95-BD4739621249}" name="Unit Sales" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{48155666-2FFE-4435-98FA-77A71F62A4CD}" name="Price" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{E6C9B305-43C4-4AA9-AF99-52F226A2A489}" name="Year Resale Value" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{53AB75B2-B4C7-4B08-A310-E333B5D08F1E}" name="Retention %" dataDxfId="70" dataCellStyle="Percent">
+    <tableColumn id="2" xr3:uid="{CCFD9DCD-33DA-4C1C-B39D-1F8C0CA940C0}" name="Manufacturer" dataDxfId="64" dataCellStyle="60% - Accent2"/>
+    <tableColumn id="1" xr3:uid="{91732ACF-B59B-4736-A06E-BE7ADB4669C2}" name="Model" dataDxfId="63" dataCellStyle="60% - Accent6"/>
+    <tableColumn id="4" xr3:uid="{AC38EB39-9FE7-4815-9A95-BD4739621249}" name="Unit Sales" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{48155666-2FFE-4435-98FA-77A71F62A4CD}" name="Price" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{E6C9B305-43C4-4AA9-AF99-52F226A2A489}" name="Year Resale Value" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{53AB75B2-B4C7-4B08-A310-E333B5D08F1E}" name="Retention %" dataDxfId="59" dataCellStyle="Percent">
       <calculatedColumnFormula>SUM(E2/D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{14C0ED08-C800-44FC-AEFF-AD4CB3BA4CE3}" name="Retention Value" dataDxfId="69" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{14C0ED08-C800-44FC-AEFF-AD4CB3BA4CE3}" name="Retention Value" dataDxfId="58" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(F2&gt;69%, "GOOD", "POOR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2D1C7A45-6CF4-4F66-812C-40A50CEEFE3C}" name="Engine Size" dataDxfId="68"/>
-    <tableColumn id="10" xr3:uid="{6F868495-C5F3-4EB0-A931-7DB5EE263B04}" name="Horsepower" dataDxfId="67"/>
-    <tableColumn id="11" xr3:uid="{21D8283C-331B-4FBC-ADCB-511EC8FEEA5B}" name="HP Level" dataDxfId="66">
+    <tableColumn id="9" xr3:uid="{2D1C7A45-6CF4-4F66-812C-40A50CEEFE3C}" name="Engine Size" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{6F868495-C5F3-4EB0-A931-7DB5EE263B04}" name="Horsepower" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{21D8283C-331B-4FBC-ADCB-511EC8FEEA5B}" name="HP Level" dataDxfId="55">
       <calculatedColumnFormula array="1">_xlfn.IFS(I2&gt;299,"High HP",I2&gt;99,"Medium HP",I2&lt;100,"Low HP")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D8DD2294-3DBB-4222-BDE1-25B41E8C6E23}" name="Vehicle_type" dataDxfId="65"/>
-    <tableColumn id="17" xr3:uid="{41974CDD-17C2-4811-8CA1-4FE62EF36874}" name="Fuel Efficiency" dataDxfId="64"/>
-    <tableColumn id="19" xr3:uid="{FF974689-EC10-4BD7-931E-F6D2FC8A04BB}" name="Power Perf Factor" dataDxfId="63"/>
-    <tableColumn id="16" xr3:uid="{A47D6D7B-55BF-4939-8425-7A7DC0E408AE}" name="Fuel Capacity" dataDxfId="62"/>
-    <tableColumn id="12" xr3:uid="{59E0B2CA-E73A-4CDD-A62F-F1A4C75E90F7}" name="Wheelbase" dataDxfId="61"/>
-    <tableColumn id="13" xr3:uid="{1318511A-327E-4603-9CFA-8A67BC21BEB8}" name="Width" dataDxfId="60"/>
-    <tableColumn id="14" xr3:uid="{B48108FE-8EF4-43AB-ACEA-F7B30A9D3C55}" name="Length" dataDxfId="59"/>
-    <tableColumn id="15" xr3:uid="{1C70CD07-6AE4-4D29-95C6-1D02DF8772F3}" name="Curb Weight" dataDxfId="58"/>
-    <tableColumn id="18" xr3:uid="{801588FA-173B-403F-BAF7-D1F66FFF62EA}" name="Latest Launch" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{D8DD2294-3DBB-4222-BDE1-25B41E8C6E23}" name="Vehicle_type" dataDxfId="54"/>
+    <tableColumn id="17" xr3:uid="{41974CDD-17C2-4811-8CA1-4FE62EF36874}" name="Fuel Efficiency" dataDxfId="53"/>
+    <tableColumn id="19" xr3:uid="{FF974689-EC10-4BD7-931E-F6D2FC8A04BB}" name="Power Perf Factor" dataDxfId="52"/>
+    <tableColumn id="16" xr3:uid="{A47D6D7B-55BF-4939-8425-7A7DC0E408AE}" name="Fuel Capacity" dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{59E0B2CA-E73A-4CDD-A62F-F1A4C75E90F7}" name="Wheelbase" dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{1318511A-327E-4603-9CFA-8A67BC21BEB8}" name="Width" dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{B48108FE-8EF4-43AB-ACEA-F7B30A9D3C55}" name="Length" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{1C70CD07-6AE4-4D29-95C6-1D02DF8772F3}" name="Curb Weight" dataDxfId="47"/>
+    <tableColumn id="18" xr3:uid="{801588FA-173B-403F-BAF7-D1F66FFF62EA}" name="Latest Launch" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D9BA20E7-01BD-4CE5-A39A-A378DD819ED1}" name="Table15" displayName="Table15" ref="A1:S156" totalsRowShown="0" headerRowDxfId="56" headerRowCellStyle="60% - Accent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D9BA20E7-01BD-4CE5-A39A-A378DD819ED1}" name="Table15" displayName="Table15" ref="A1:S156" totalsRowShown="0" headerRowDxfId="45" headerRowCellStyle="60% - Accent1">
   <autoFilter ref="A1:S156" xr:uid="{142A1155-8F99-4580-8274-3FFCD265F860}">
     <filterColumn colId="0">
       <filters>
@@ -12334,65 +12301,65 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="2" xr3:uid="{5BFF9CA1-D18F-48F8-B139-C94FCAB0E175}" name="Manufacturer" dataDxfId="55" dataCellStyle="60% - Accent2"/>
-    <tableColumn id="1" xr3:uid="{43B3A4A3-6CC5-4B1F-9BA5-697A4F09A487}" name="Model" dataDxfId="54" dataCellStyle="60% - Accent6"/>
-    <tableColumn id="19" xr3:uid="{5B90FD03-F436-4395-9630-5BC3AE66755A}" name="Power Perf Factor" dataDxfId="53" dataCellStyle="60% - Accent6"/>
-    <tableColumn id="4" xr3:uid="{2F98F040-7842-4713-AEFE-12CD948B81ED}" name="Unit Sales" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{6A58B398-9B8D-495F-8939-B398B67C09F9}" name="Price" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{CFBD5404-82BE-457B-8590-AD11A6B7EF8F}" name="Year Resale Value" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{7684E2FD-1B7C-4F58-8E02-AB765C88FB13}" name="Retention %" dataDxfId="49" dataCellStyle="Percent">
+    <tableColumn id="2" xr3:uid="{5BFF9CA1-D18F-48F8-B139-C94FCAB0E175}" name="Manufacturer" dataDxfId="44" dataCellStyle="60% - Accent2"/>
+    <tableColumn id="1" xr3:uid="{43B3A4A3-6CC5-4B1F-9BA5-697A4F09A487}" name="Model" dataDxfId="43" dataCellStyle="60% - Accent6"/>
+    <tableColumn id="19" xr3:uid="{5B90FD03-F436-4395-9630-5BC3AE66755A}" name="Power Perf Factor" dataDxfId="42" dataCellStyle="60% - Accent6"/>
+    <tableColumn id="4" xr3:uid="{2F98F040-7842-4713-AEFE-12CD948B81ED}" name="Unit Sales" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{6A58B398-9B8D-495F-8939-B398B67C09F9}" name="Price" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{CFBD5404-82BE-457B-8590-AD11A6B7EF8F}" name="Year Resale Value" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{7684E2FD-1B7C-4F58-8E02-AB765C88FB13}" name="Retention %" dataDxfId="38" dataCellStyle="Percent">
       <calculatedColumnFormula>SUM(F2/E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4F26BE56-C2D9-44F3-86FD-D2945E0358C0}" name="Retention Value" dataDxfId="48" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{4F26BE56-C2D9-44F3-86FD-D2945E0358C0}" name="Retention Value" dataDxfId="37" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(G2&gt;69%, "GOOD", "POOR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E2821A61-E719-4923-891A-BCFDE42F66D0}" name="Engine Size" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{16623E42-D7B5-47C4-B7B5-265380D2ACB5}" name="Horsepower" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{D6BC5B95-B4B5-4D2C-B442-659931E923AB}" name="HP Level" dataDxfId="45">
+    <tableColumn id="9" xr3:uid="{E2821A61-E719-4923-891A-BCFDE42F66D0}" name="Engine Size" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{16623E42-D7B5-47C4-B7B5-265380D2ACB5}" name="Horsepower" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{D6BC5B95-B4B5-4D2C-B442-659931E923AB}" name="HP Level" dataDxfId="34">
       <calculatedColumnFormula array="1">_xlfn.IFS(J2&gt;299,"High HP",J2&gt;99,"Medium HP",J2&lt;100,"Low HP")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D89FC93A-602D-4147-B5D8-052BD3AAEFA9}" name="Vehicle_type" dataDxfId="44"/>
-    <tableColumn id="17" xr3:uid="{09BC724F-FE73-4569-B3C5-F0F8A6DB4C85}" name="Fuel Efficiency" dataDxfId="43" dataCellStyle="60% - Accent6"/>
-    <tableColumn id="12" xr3:uid="{55924A29-F156-4CD0-8425-CED32C98068B}" name="Wheelbase" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{56DEB4B4-962C-464A-8CF0-5AF892D29D15}" name="Width" dataDxfId="41"/>
-    <tableColumn id="14" xr3:uid="{1EDAA041-E793-4BBE-B154-A3806B225DA4}" name="Length" dataDxfId="40"/>
-    <tableColumn id="15" xr3:uid="{8B517A00-9F46-45B8-851E-0C41E81C7F5A}" name="Curb Weight" dataDxfId="39"/>
-    <tableColumn id="16" xr3:uid="{C0D2D5B9-1522-4D17-A522-05AF3FA10469}" name="Fuel Capacity" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{8890314F-1652-4E10-ABA4-284B9415484A}" name="Latest Launch" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{D89FC93A-602D-4147-B5D8-052BD3AAEFA9}" name="Vehicle_type" dataDxfId="33"/>
+    <tableColumn id="17" xr3:uid="{09BC724F-FE73-4569-B3C5-F0F8A6DB4C85}" name="Fuel Efficiency" dataDxfId="32" dataCellStyle="60% - Accent6"/>
+    <tableColumn id="12" xr3:uid="{55924A29-F156-4CD0-8425-CED32C98068B}" name="Wheelbase" dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{56DEB4B4-962C-464A-8CF0-5AF892D29D15}" name="Width" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{1EDAA041-E793-4BBE-B154-A3806B225DA4}" name="Length" dataDxfId="29"/>
+    <tableColumn id="15" xr3:uid="{8B517A00-9F46-45B8-851E-0C41E81C7F5A}" name="Curb Weight" dataDxfId="28"/>
+    <tableColumn id="16" xr3:uid="{C0D2D5B9-1522-4D17-A522-05AF3FA10469}" name="Fuel Capacity" dataDxfId="27"/>
+    <tableColumn id="18" xr3:uid="{8890314F-1652-4E10-ABA4-284B9415484A}" name="Latest Launch" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{597DCCBB-1D00-4B74-A561-F0C0BDE98FA1}" name="Table1" displayName="Table1" ref="A1:S156" totalsRowShown="0" headerRowDxfId="36" headerRowCellStyle="60% - Accent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{597DCCBB-1D00-4B74-A561-F0C0BDE98FA1}" name="Table1" displayName="Table1" ref="A1:S156" totalsRowShown="0" headerRowDxfId="25" headerRowCellStyle="60% - Accent1">
   <autoFilter ref="A1:S156" xr:uid="{142A1155-8F99-4580-8274-3FFCD265F860}"/>
   <tableColumns count="19">
-    <tableColumn id="2" xr3:uid="{0090DD31-AAEF-418B-A6D5-5A47F973884A}" name="Manufacturer" dataDxfId="35" dataCellStyle="60% - Accent2"/>
-    <tableColumn id="1" xr3:uid="{1D457C4B-D2B8-4760-9FBD-20980339C812}" name="Model" dataDxfId="34" dataCellStyle="60% - Accent6"/>
-    <tableColumn id="4" xr3:uid="{8522711B-6353-4D72-9921-4036DEB24699}" name="Unit Sales" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{3F2EFF05-CEC1-43C4-8457-EC0A04BFE37D}" name="Price" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{D0C7E9A3-6A78-4834-995F-71A07F7E5FEC}" name="Year Resale Value" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{2892AE5C-2583-41F9-9297-9EA4C2895B5F}" name="Retention %" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="2" xr3:uid="{0090DD31-AAEF-418B-A6D5-5A47F973884A}" name="Manufacturer" dataDxfId="24" dataCellStyle="60% - Accent2"/>
+    <tableColumn id="1" xr3:uid="{1D457C4B-D2B8-4760-9FBD-20980339C812}" name="Model" dataDxfId="23" dataCellStyle="60% - Accent6"/>
+    <tableColumn id="4" xr3:uid="{8522711B-6353-4D72-9921-4036DEB24699}" name="Unit Sales" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{3F2EFF05-CEC1-43C4-8457-EC0A04BFE37D}" name="Price" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{D0C7E9A3-6A78-4834-995F-71A07F7E5FEC}" name="Year Resale Value" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{2892AE5C-2583-41F9-9297-9EA4C2895B5F}" name="Retention %" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>SUM(E2/D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{40A7E790-705B-474C-BD5E-B93CFDEAAD37}" name="Retention Value" dataDxfId="29" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{40A7E790-705B-474C-BD5E-B93CFDEAAD37}" name="Retention Value" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(F2&gt;69%, "GOOD", "POOR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9FD1D782-0EB9-4AC8-9FB6-1F5437BC6100}" name="Engine Size" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{97F7DE8D-9589-426B-AA4F-2E3F8BB7A81B}" name="Horsepower" dataDxfId="27"/>
-    <tableColumn id="11" xr3:uid="{4CB9C68E-A6F1-497A-9877-E41495059145}" name="HP Level" dataDxfId="26">
+    <tableColumn id="9" xr3:uid="{9FD1D782-0EB9-4AC8-9FB6-1F5437BC6100}" name="Engine Size" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{97F7DE8D-9589-426B-AA4F-2E3F8BB7A81B}" name="Horsepower" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{4CB9C68E-A6F1-497A-9877-E41495059145}" name="HP Level" dataDxfId="15">
       <calculatedColumnFormula array="1">_xlfn.IFS(I2&gt;299,"High HP",I2&gt;99,"Medium HP",I2&lt;100,"Low HP")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3733B2DD-D65D-439A-9EC2-28F65DC369D7}" name="Vehicle_type" dataDxfId="25"/>
-    <tableColumn id="17" xr3:uid="{5136D0F0-2F8F-4D70-995F-CE39B1996127}" name="Fuel Efficiency" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{5F133F36-F1C6-453A-A10C-A9917A623804}" name="Power Perf Factor" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{6E551230-1170-40DA-8649-BDDA922271D8}" name="Wheelbase" dataDxfId="22"/>
-    <tableColumn id="13" xr3:uid="{53A36FF3-E823-43B4-958B-9E02EC2B56F7}" name="Width" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{0728B768-EB40-4E54-9F8B-8FC310D3272C}" name="Length" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{2264EB11-0818-4B2A-A027-42B066FA9869}" name="Curb Weight" dataDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{58B24934-BE7E-4FBD-9F96-CEF0725C6117}" name="Fuel Capacity" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{00FF364F-DDBE-4E2C-8F3E-DBDA321FA22A}" name="Latest Launch" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{3733B2DD-D65D-439A-9EC2-28F65DC369D7}" name="Vehicle_type" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{5136D0F0-2F8F-4D70-995F-CE39B1996127}" name="Fuel Efficiency" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{5F133F36-F1C6-453A-A10C-A9917A623804}" name="Power Perf Factor" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{6E551230-1170-40DA-8649-BDDA922271D8}" name="Wheelbase" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{53A36FF3-E823-43B4-958B-9E02EC2B56F7}" name="Width" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{0728B768-EB40-4E54-9F8B-8FC310D3272C}" name="Length" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{2264EB11-0818-4B2A-A027-42B066FA9869}" name="Curb Weight" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{58B24934-BE7E-4FBD-9F96-CEF0725C6117}" name="Fuel Capacity" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{00FF364F-DDBE-4E2C-8F3E-DBDA321FA22A}" name="Latest Launch" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12698,7 +12665,7 @@
   <dimension ref="A3:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:O24"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22869,10 +22836,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G156">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="POOR">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="POOR">
       <formula>NOT(ISERROR(SEARCH("POOR",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="GOOD">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="GOOD">
       <formula>NOT(ISERROR(SEARCH("GOOD",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32608,10 +32575,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H156">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="POOR">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="POOR">
       <formula>NOT(ISERROR(SEARCH("POOR",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="GOOD">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="GOOD">
       <formula>NOT(ISERROR(SEARCH("GOOD",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42348,10 +42315,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G156">
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="POOR">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="POOR">
       <formula>NOT(ISERROR(SEARCH("POOR",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="GOOD">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="GOOD">
       <formula>NOT(ISERROR(SEARCH("GOOD",G2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>